<commit_message>
Update results with T2D samples
</commit_message>
<xml_diff>
--- a/00_Data/SampleList.xlsx
+++ b/00_Data/SampleList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/mathieu_simon_unibe_ch/Documents/FABTIB/00_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:9_{99E2AE50-C5F7-E446-9B85-37C5075ADC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DADCD7E9-8F8F-4376-A8D6-CDD137C616D8}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="13_ncr:9_{99E2AE50-C5F7-E446-9B85-37C5075ADC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA93EF1-0F26-4C44-93B4-894CAC4D8F85}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{E913811A-4AD7-CA48-9433-D824E84D6F4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="121">
   <si>
     <t>C0014618</t>
   </si>
@@ -312,6 +312,93 @@
   </si>
   <si>
     <t>Group (T2D or Ctrl)</t>
+  </si>
+  <si>
+    <t>C0020950</t>
+  </si>
+  <si>
+    <t>C0020969</t>
+  </si>
+  <si>
+    <t>C0020970</t>
+  </si>
+  <si>
+    <t>C0020971</t>
+  </si>
+  <si>
+    <t>C0021051</t>
+  </si>
+  <si>
+    <t>C0021057</t>
+  </si>
+  <si>
+    <t>C0023223</t>
+  </si>
+  <si>
+    <t>C0023247</t>
+  </si>
+  <si>
+    <t>C0023340</t>
+  </si>
+  <si>
+    <t>C0023343</t>
+  </si>
+  <si>
+    <t>C0023364</t>
+  </si>
+  <si>
+    <t>C0023381</t>
+  </si>
+  <si>
+    <t>C0023451</t>
+  </si>
+  <si>
+    <t>C0023452</t>
+  </si>
+  <si>
+    <t>C0023511</t>
+  </si>
+  <si>
+    <t>C0023688</t>
+  </si>
+  <si>
+    <t>C0024065</t>
+  </si>
+  <si>
+    <t>C0024066</t>
+  </si>
+  <si>
+    <t>C0024090</t>
+  </si>
+  <si>
+    <t>C0024091</t>
+  </si>
+  <si>
+    <t>C0024093</t>
+  </si>
+  <si>
+    <t>C0024264</t>
+  </si>
+  <si>
+    <t>C0024273</t>
+  </si>
+  <si>
+    <t>C0024275</t>
+  </si>
+  <si>
+    <t>C0020829</t>
+  </si>
+  <si>
+    <t>C0020931</t>
+  </si>
+  <si>
+    <t>C0024278</t>
+  </si>
+  <si>
+    <t>C0024282</t>
+  </si>
+  <si>
+    <t>C0024330</t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1529,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}" name="Tableau1" displayName="Tableau1" ref="A1:L32" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:L32" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}" name="Tableau1" displayName="Tableau1" ref="A1:L61" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:L61" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EFE0719B-71AF-45A2-9C0C-F06955FA71D2}" name="Filename" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{A9D459DD-C430-497C-9694-4E8E36446451}" name="Specimen ID" dataDxfId="28"/>
@@ -1783,7 +1870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61F126B-3880-3249-A743-AEAED9A190C5}">
   <dimension ref="A1:AG67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -3324,7 +3413,22 @@
       <c r="U32" s="6"/>
       <c r="V32" s="7"/>
     </row>
-    <row r="33" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -3346,7 +3450,22 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="4"/>
     </row>
-    <row r="34" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -3368,7 +3487,22 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="4"/>
     </row>
-    <row r="35" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -3380,7 +3514,22 @@
       <c r="U35" s="6"/>
       <c r="V35" s="4"/>
     </row>
-    <row r="36" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -3402,7 +3551,22 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="4"/>
     </row>
-    <row r="37" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -3424,7 +3588,22 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="4"/>
     </row>
-    <row r="38" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -3446,7 +3625,22 @@
       <c r="AF38" s="6"/>
       <c r="AG38" s="4"/>
     </row>
-    <row r="39" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -3468,7 +3662,22 @@
       <c r="AF39" s="6"/>
       <c r="AG39" s="7"/>
     </row>
-    <row r="40" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
@@ -3490,7 +3699,22 @@
       <c r="AF40" s="6"/>
       <c r="AG40" s="4"/>
     </row>
-    <row r="41" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -3512,7 +3736,22 @@
       <c r="AF41" s="6"/>
       <c r="AG41" s="4"/>
     </row>
-    <row r="42" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -3534,7 +3773,22 @@
       <c r="AF42" s="6"/>
       <c r="AG42" s="4"/>
     </row>
-    <row r="43" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A43" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -3556,7 +3810,22 @@
       <c r="AF43" s="6"/>
       <c r="AG43" s="4"/>
     </row>
-    <row r="44" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -3578,7 +3847,22 @@
       <c r="AF44" s="6"/>
       <c r="AG44" s="4"/>
     </row>
-    <row r="45" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="4"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
@@ -3600,7 +3884,22 @@
       <c r="AF45" s="6"/>
       <c r="AG45" s="4"/>
     </row>
-    <row r="46" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A46" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -3622,7 +3921,22 @@
       <c r="AF46" s="6"/>
       <c r="AG46" s="4"/>
     </row>
-    <row r="47" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I47" s="4"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -3644,7 +3958,22 @@
       <c r="AF47" s="6"/>
       <c r="AG47" s="4"/>
     </row>
-    <row r="48" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A48" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -3666,7 +3995,22 @@
       <c r="AF48" s="6"/>
       <c r="AG48" s="4"/>
     </row>
-    <row r="49" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A49" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
@@ -3688,7 +4032,22 @@
       <c r="AF49" s="6"/>
       <c r="AG49" s="4"/>
     </row>
-    <row r="50" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
@@ -3710,7 +4069,22 @@
       <c r="AF50" s="6"/>
       <c r="AG50" s="4"/>
     </row>
-    <row r="51" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
@@ -3722,7 +4096,22 @@
       <c r="U51" s="6"/>
       <c r="V51" s="7"/>
     </row>
-    <row r="52" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A52" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I52" s="4"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -3744,7 +4133,22 @@
       <c r="AF52" s="6"/>
       <c r="AG52" s="4"/>
     </row>
-    <row r="53" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A53" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I53" s="4"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
@@ -3766,7 +4170,22 @@
       <c r="AF53" s="6"/>
       <c r="AG53" s="4"/>
     </row>
-    <row r="54" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
@@ -3788,7 +4207,22 @@
       <c r="AF54" s="6"/>
       <c r="AG54" s="7"/>
     </row>
-    <row r="55" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A55" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I55" s="4"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
@@ -3810,7 +4244,22 @@
       <c r="AF55" s="6"/>
       <c r="AG55" s="4"/>
     </row>
-    <row r="56" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A56" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I56" s="4"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
@@ -3832,7 +4281,22 @@
       <c r="AF56" s="6"/>
       <c r="AG56" s="4"/>
     </row>
-    <row r="57" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A57" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I57" s="4"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -3854,7 +4318,22 @@
       <c r="AF57" s="6"/>
       <c r="AG57" s="4"/>
     </row>
-    <row r="58" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A58" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I58" s="4"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
@@ -3876,7 +4355,22 @@
       <c r="AF58" s="6"/>
       <c r="AG58" s="4"/>
     </row>
-    <row r="59" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I59" s="4"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -3888,7 +4382,22 @@
       <c r="U59" s="6"/>
       <c r="V59" s="4"/>
     </row>
-    <row r="60" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A60" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -3910,7 +4419,22 @@
       <c r="AF60" s="6"/>
       <c r="AG60" s="4"/>
     </row>
-    <row r="61" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A61" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I61" s="4"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -3922,7 +4446,7 @@
       <c r="U61" s="6"/>
       <c r="V61" s="4"/>
     </row>
-    <row r="62" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.5">
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -3934,7 +4458,7 @@
       <c r="U62" s="6"/>
       <c r="V62" s="4"/>
     </row>
-    <row r="63" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.5">
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
@@ -3946,7 +4470,7 @@
       <c r="U63" s="6"/>
       <c r="V63" s="7"/>
     </row>
-    <row r="64" spans="13:33" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.5">
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>

</xml_diff>

<commit_message>
Add new control samples
</commit_message>
<xml_diff>
--- a/00_Data/SampleList.xlsx
+++ b/00_Data/SampleList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/mathieu_simon_unibe_ch/Documents/FABTIB/00_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="13_ncr:9_{99E2AE50-C5F7-E446-9B85-37C5075ADC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA93EF1-0F26-4C44-93B4-894CAC4D8F85}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="13_ncr:9_{99E2AE50-C5F7-E446-9B85-37C5075ADC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3D70D44-3036-47AB-A8AD-8453DE5AB5CB}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{E913811A-4AD7-CA48-9433-D824E84D6F4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="149">
   <si>
     <t>C0014618</t>
   </si>
@@ -399,6 +399,90 @@
   </si>
   <si>
     <t>C0024330</t>
+  </si>
+  <si>
+    <t>C0024276</t>
+  </si>
+  <si>
+    <t>C0024269</t>
+  </si>
+  <si>
+    <t>C0024268</t>
+  </si>
+  <si>
+    <t>C0024267</t>
+  </si>
+  <si>
+    <t>C0024262</t>
+  </si>
+  <si>
+    <t>C0024094</t>
+  </si>
+  <si>
+    <t>C0024067</t>
+  </si>
+  <si>
+    <t>C0024064</t>
+  </si>
+  <si>
+    <t>C0023986</t>
+  </si>
+  <si>
+    <t>C0023689</t>
+  </si>
+  <si>
+    <t>C0023676</t>
+  </si>
+  <si>
+    <t>C0023512</t>
+  </si>
+  <si>
+    <t>C0023380</t>
+  </si>
+  <si>
+    <t>C0023369</t>
+  </si>
+  <si>
+    <t>C0023367</t>
+  </si>
+  <si>
+    <t>C0023365</t>
+  </si>
+  <si>
+    <t>C0023344</t>
+  </si>
+  <si>
+    <t>C0023342</t>
+  </si>
+  <si>
+    <t>C0023248</t>
+  </si>
+  <si>
+    <t>C0023224</t>
+  </si>
+  <si>
+    <t>C0023217</t>
+  </si>
+  <si>
+    <t>C0021055</t>
+  </si>
+  <si>
+    <t>C0020968</t>
+  </si>
+  <si>
+    <t>C0020967</t>
+  </si>
+  <si>
+    <t>C0020966</t>
+  </si>
+  <si>
+    <t>C0020965</t>
+  </si>
+  <si>
+    <t>C0020953</t>
+  </si>
+  <si>
+    <t>C0020952</t>
   </si>
 </sst>
 </file>
@@ -1529,8 +1613,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}" name="Tableau1" displayName="Tableau1" ref="A1:L61" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:L61" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}" name="Tableau1" displayName="Tableau1" ref="A1:L89" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:L89" xr:uid="{C9238200-1F5D-457F-9011-A37A5DC3E7F2}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EFE0719B-71AF-45A2-9C0C-F06955FA71D2}" name="Filename" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{A9D459DD-C430-497C-9694-4E8E36446451}" name="Specimen ID" dataDxfId="28"/>
@@ -1868,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61F126B-3880-3249-A743-AEAED9A190C5}">
-  <dimension ref="A1:AG67"/>
+  <dimension ref="A1:AG89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4447,6 +4531,21 @@
       <c r="V61" s="4"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I62" s="4"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -4459,6 +4558,21 @@
       <c r="V62" s="4"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A63" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I63" s="4"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
@@ -4471,6 +4585,21 @@
       <c r="V63" s="7"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.5">
+      <c r="A64" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" s="4"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
@@ -4482,7 +4611,22 @@
       <c r="U64" s="6"/>
       <c r="V64" s="4"/>
     </row>
-    <row r="65" spans="13:22" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A65" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I65" s="4"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
@@ -4494,7 +4638,22 @@
       <c r="U65" s="6"/>
       <c r="V65" s="7"/>
     </row>
-    <row r="66" spans="13:22" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A66" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
@@ -4506,7 +4665,22 @@
       <c r="U66" s="6"/>
       <c r="V66" s="4"/>
     </row>
-    <row r="67" spans="13:22" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A67" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
@@ -4517,6 +4691,380 @@
       <c r="T67" s="5"/>
       <c r="U67" s="6"/>
       <c r="V67" s="4"/>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A68" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I68" s="4"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="4"/>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A69" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="4"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A70" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I71" s="4"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="4"/>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A72" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I72" s="4"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="4"/>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A73" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I73" s="4"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="4"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A74" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I74" s="4"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="4"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A75" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I75" s="4"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="4"/>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A76" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I76" s="4"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A77" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I77" s="4"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="4"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A78" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I78" s="4"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="4"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A79" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I79" s="4"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="4"/>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A80" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I80" s="4"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="4"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A81" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I81" s="4"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="4"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A82" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I82" s="4"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="4"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A83" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I83" s="4"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="4"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A84" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I84" s="4"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="4"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A85" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I85" s="4"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="4"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A86" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I86" s="4"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="4"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A87" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I87" s="4"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="4"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A88" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I88" s="4"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="4"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A89" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I89" s="4"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K32">

</xml_diff>